<commit_message>
Address code review feedback - improve compatibility and maintainability
Co-authored-by: aliabdelaal-adm <233267419+aliabdelaal-adm@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/pet-shops-by-area.xlsx
+++ b/pet-shops-by-area.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="📊 الملخص - Summary" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Summary - الملخص" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="آل نهيان" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="الباهية" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="البطين" sheetId="4" state="visible" r:id="rId4"/>
@@ -642,7 +642,7 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>تاريخ الإنشاء: 2025-12-09 06:53</t>
+          <t>تاريخ الإنشاء: 2025-12-09 06:56</t>
         </is>
       </c>
     </row>
@@ -697,7 +697,7 @@
       </c>
       <c r="E7" s="6" t="inlineStr">
         <is>
-          <t>🔴 كبير جداً</t>
+          <t>كبير جداً - Very Large</t>
         </is>
       </c>
       <c r="F7" s="5" t="inlineStr">
@@ -725,7 +725,7 @@
       </c>
       <c r="E8" s="7" t="inlineStr">
         <is>
-          <t>🟡 كبير</t>
+          <t>كبير - Large</t>
         </is>
       </c>
       <c r="F8" s="5" t="inlineStr">
@@ -753,7 +753,7 @@
       </c>
       <c r="E9" s="7" t="inlineStr">
         <is>
-          <t>🟡 كبير</t>
+          <t>كبير - Large</t>
         </is>
       </c>
       <c r="F9" s="5" t="inlineStr">
@@ -781,7 +781,7 @@
       </c>
       <c r="E10" s="7" t="inlineStr">
         <is>
-          <t>🟡 كبير</t>
+          <t>كبير - Large</t>
         </is>
       </c>
       <c r="F10" s="5" t="inlineStr">
@@ -809,7 +809,7 @@
       </c>
       <c r="E11" s="7" t="inlineStr">
         <is>
-          <t>🟡 كبير</t>
+          <t>كبير - Large</t>
         </is>
       </c>
       <c r="F11" s="5" t="inlineStr">
@@ -837,7 +837,7 @@
       </c>
       <c r="E12" s="7" t="inlineStr">
         <is>
-          <t>🟡 كبير</t>
+          <t>كبير - Large</t>
         </is>
       </c>
       <c r="F12" s="5" t="inlineStr">
@@ -865,7 +865,7 @@
       </c>
       <c r="E13" s="7" t="inlineStr">
         <is>
-          <t>🟡 كبير</t>
+          <t>كبير - Large</t>
         </is>
       </c>
       <c r="F13" s="5" t="inlineStr">
@@ -893,7 +893,7 @@
       </c>
       <c r="E14" s="7" t="inlineStr">
         <is>
-          <t>🟡 كبير</t>
+          <t>كبير - Large</t>
         </is>
       </c>
       <c r="F14" s="5" t="inlineStr">
@@ -921,7 +921,7 @@
       </c>
       <c r="E15" s="7" t="inlineStr">
         <is>
-          <t>🟡 كبير</t>
+          <t>كبير - Large</t>
         </is>
       </c>
       <c r="F15" s="5" t="inlineStr">
@@ -949,7 +949,7 @@
       </c>
       <c r="E16" s="8" t="inlineStr">
         <is>
-          <t>🟢 متوسط</t>
+          <t>متوسط - Medium</t>
         </is>
       </c>
       <c r="F16" s="5" t="inlineStr">
@@ -977,7 +977,7 @@
       </c>
       <c r="E17" s="8" t="inlineStr">
         <is>
-          <t>🟢 متوسط</t>
+          <t>متوسط - Medium</t>
         </is>
       </c>
       <c r="F17" s="5" t="inlineStr">
@@ -1005,7 +1005,7 @@
       </c>
       <c r="E18" s="8" t="inlineStr">
         <is>
-          <t>🟢 متوسط</t>
+          <t>متوسط - Medium</t>
         </is>
       </c>
       <c r="F18" s="5" t="inlineStr">
@@ -1033,7 +1033,7 @@
       </c>
       <c r="E19" s="8" t="inlineStr">
         <is>
-          <t>🟢 متوسط</t>
+          <t>متوسط - Medium</t>
         </is>
       </c>
       <c r="F19" s="5" t="inlineStr">
@@ -1061,7 +1061,7 @@
       </c>
       <c r="E20" s="8" t="inlineStr">
         <is>
-          <t>🟢 متوسط</t>
+          <t>متوسط - Medium</t>
         </is>
       </c>
       <c r="F20" s="5" t="inlineStr">
@@ -1089,7 +1089,7 @@
       </c>
       <c r="E21" s="9" t="inlineStr">
         <is>
-          <t>🔵 صغير</t>
+          <t>صغير - Small</t>
         </is>
       </c>
       <c r="F21" s="5" t="inlineStr">
@@ -1117,7 +1117,7 @@
       </c>
       <c r="E22" s="9" t="inlineStr">
         <is>
-          <t>🔵 صغير</t>
+          <t>صغير - Small</t>
         </is>
       </c>
       <c r="F22" s="5" t="inlineStr">
@@ -1145,7 +1145,7 @@
       </c>
       <c r="E23" s="9" t="inlineStr">
         <is>
-          <t>🔵 صغير</t>
+          <t>صغير - Small</t>
         </is>
       </c>
       <c r="F23" s="5" t="inlineStr">
@@ -1173,7 +1173,7 @@
       </c>
       <c r="E24" s="9" t="inlineStr">
         <is>
-          <t>🔵 صغير</t>
+          <t>صغير - Small</t>
         </is>
       </c>
       <c r="F24" s="5" t="inlineStr">
@@ -1201,7 +1201,7 @@
       </c>
       <c r="E25" s="9" t="inlineStr">
         <is>
-          <t>🔵 صغير</t>
+          <t>صغير - Small</t>
         </is>
       </c>
       <c r="F25" s="5" t="inlineStr">
@@ -1229,7 +1229,7 @@
       </c>
       <c r="E26" s="9" t="inlineStr">
         <is>
-          <t>🔵 صغير</t>
+          <t>صغير - Small</t>
         </is>
       </c>
       <c r="F26" s="5" t="inlineStr">
@@ -1257,7 +1257,7 @@
       </c>
       <c r="E27" s="9" t="inlineStr">
         <is>
-          <t>🔵 صغير</t>
+          <t>صغير - Small</t>
         </is>
       </c>
       <c r="F27" s="5" t="inlineStr">
@@ -1285,7 +1285,7 @@
       </c>
       <c r="E28" s="9" t="inlineStr">
         <is>
-          <t>🔵 صغير</t>
+          <t>صغير - Small</t>
         </is>
       </c>
       <c r="F28" s="5" t="inlineStr">
@@ -1313,7 +1313,7 @@
       </c>
       <c r="E29" s="9" t="inlineStr">
         <is>
-          <t>🔵 صغير</t>
+          <t>صغير - Small</t>
         </is>
       </c>
       <c r="F29" s="5" t="inlineStr">
@@ -1341,7 +1341,7 @@
       </c>
       <c r="E30" s="9" t="inlineStr">
         <is>
-          <t>🔵 صغير</t>
+          <t>صغير - Small</t>
         </is>
       </c>
       <c r="F30" s="5" t="inlineStr">
@@ -1369,7 +1369,7 @@
       </c>
       <c r="E31" s="9" t="inlineStr">
         <is>
-          <t>🔵 صغير</t>
+          <t>صغير - Small</t>
         </is>
       </c>
       <c r="F31" s="5" t="inlineStr">
@@ -1397,7 +1397,7 @@
       </c>
       <c r="E32" s="9" t="inlineStr">
         <is>
-          <t>🔵 صغير</t>
+          <t>صغير - Small</t>
         </is>
       </c>
       <c r="F32" s="5" t="inlineStr">

</xml_diff>